<commit_message>
Add ROLE and ACTOR_AWARD datasets
</commit_message>
<xml_diff>
--- a/movies.xlsx
+++ b/movies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johann Wagner\Documents\GitHub\comp2400\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACBD6AD-FAE4-438E-8839-7660436000ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0579696D-A9B9-44A4-8779-E384413B608A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24800" windowHeight="14620" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24800" windowHeight="14620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MOVIE" sheetId="3" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="RESTRICTION" sheetId="11" r:id="rId10"/>
     <sheet name="WRITER_AWARD" sheetId="12" r:id="rId11"/>
     <sheet name="DIRECTOR_AWARD" sheetId="13" r:id="rId12"/>
+    <sheet name="ACTOR_AWARD" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5211" uniqueCount="1755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5413" uniqueCount="1780">
   <si>
     <t>id</t>
   </si>
@@ -5312,6 +5313,81 @@
   </si>
   <si>
     <t>BestDirector</t>
+  </si>
+  <si>
+    <t>bestactorinasupportingrole</t>
+  </si>
+  <si>
+    <t>Bestactorinaleadingrole</t>
+  </si>
+  <si>
+    <t>ActorinaLeadingRole</t>
+  </si>
+  <si>
+    <t>Won</t>
+  </si>
+  <si>
+    <t>ActorinasupportingRole</t>
+  </si>
+  <si>
+    <t>ActressinasupportingRole</t>
+  </si>
+  <si>
+    <t>ActressinaLeadingRole</t>
+  </si>
+  <si>
+    <t>BestActor</t>
+  </si>
+  <si>
+    <t>BestActress</t>
+  </si>
+  <si>
+    <t>BestsupportingActress</t>
+  </si>
+  <si>
+    <t>BestActressinaleadrole</t>
+  </si>
+  <si>
+    <t>BestActorinaleadrole</t>
+  </si>
+  <si>
+    <t>BestActressinasupportingrole</t>
+  </si>
+  <si>
+    <t>BestActorinasupportingrole</t>
+  </si>
+  <si>
+    <t>BestSupportingActress</t>
+  </si>
+  <si>
+    <t>BestSupportingActor</t>
+  </si>
+  <si>
+    <t>BestPerformancebyanActress</t>
+  </si>
+  <si>
+    <t>BestActorinaLeadingRole</t>
+  </si>
+  <si>
+    <t>BestPerformancebyanActor</t>
+  </si>
+  <si>
+    <t>ActoroftheYear</t>
+  </si>
+  <si>
+    <t>BestActressinaSupportingRole</t>
+  </si>
+  <si>
+    <t>ActorOFtheYear</t>
+  </si>
+  <si>
+    <t>BestActressinaLeadingRole</t>
+  </si>
+  <si>
+    <t>BestActorinaSupportingRole</t>
+  </si>
+  <si>
+    <t>BestActorSupporting</t>
   </si>
 </sst>
 </file>
@@ -5774,7 +5850,7 @@
   <dimension ref="A1:E103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15255,7 +15331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F515F3-0F8A-46EF-BD5E-692510D411A3}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
@@ -15418,6 +15494,941 @@
         <v>1754</v>
       </c>
       <c r="F8" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D1F313-EE70-422D-8CC2-A392837DE898}">
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>896</v>
+      </c>
+      <c r="B1" t="s">
+        <v>897</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1742</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1743</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B2">
+        <v>2000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E2">
+        <v>2001</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1755</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B3">
+        <v>2000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1572</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E3">
+        <v>2001</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1756</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>986</v>
+      </c>
+      <c r="B4">
+        <v>1997</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1477</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E4">
+        <v>1998</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1757</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>985</v>
+      </c>
+      <c r="B5">
+        <v>1997</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1476</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E5">
+        <v>1998</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1759</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>980</v>
+      </c>
+      <c r="B6">
+        <v>1998</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E6">
+        <v>1998</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1760</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>988</v>
+      </c>
+      <c r="B7">
+        <v>1999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1479</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E7">
+        <v>1999</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1761</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>984</v>
+      </c>
+      <c r="B8">
+        <v>1999</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1469</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E8">
+        <v>1999</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1757</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>981</v>
+      </c>
+      <c r="B9">
+        <v>1999</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E9">
+        <v>1999</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1759</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>999</v>
+      </c>
+      <c r="B10">
+        <v>1997</v>
+      </c>
+      <c r="C10" t="s">
+        <v>788</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E10">
+        <v>1999</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1762</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B11">
+        <v>1993</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1515</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E11">
+        <v>1994</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1763</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B12">
+        <v>1993</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1517</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E12">
+        <v>1994</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1764</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B13">
+        <v>1993</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1515</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E13">
+        <v>1993</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1765</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B14">
+        <v>1993</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E14">
+        <v>1993</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1766</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B15">
+        <v>1993</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1515</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E15">
+        <v>1994</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1765</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B16">
+        <v>1992</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E16">
+        <v>1992</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1767</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B17">
+        <v>1992</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1523</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E17">
+        <v>1992</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1768</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B18">
+        <v>2000</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E18">
+        <v>2001</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1768</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B19">
+        <v>2000</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E19">
+        <v>2001</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1762</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>978</v>
+      </c>
+      <c r="B20">
+        <v>1960</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E20">
+        <v>1961</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1769</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>915</v>
+      </c>
+      <c r="B21">
+        <v>1995</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1616</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E21">
+        <v>1996</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1770</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>920</v>
+      </c>
+      <c r="B22">
+        <v>1990</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1623</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E22">
+        <v>1991</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1771</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>476</v>
+      </c>
+      <c r="B23">
+        <v>1992</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1632</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E23">
+        <v>1993</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1772</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>476</v>
+      </c>
+      <c r="B24">
+        <v>1992</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1632</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E24">
+        <v>1993</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1762</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>476</v>
+      </c>
+      <c r="B25">
+        <v>1992</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1632</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E25">
+        <v>1993</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1773</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>476</v>
+      </c>
+      <c r="B26">
+        <v>1992</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1633</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E26">
+        <v>1993</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1771</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>476</v>
+      </c>
+      <c r="B27">
+        <v>1992</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1632</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E27">
+        <v>1993</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>926</v>
+      </c>
+      <c r="B28">
+        <v>1993</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1637</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E28">
+        <v>1994</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1775</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>926</v>
+      </c>
+      <c r="B29">
+        <v>1993</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1637</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E29">
+        <v>1994</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1775</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>935</v>
+      </c>
+      <c r="B30">
+        <v>1990</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1654</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E30">
+        <v>1991</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1772</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>935</v>
+      </c>
+      <c r="B31">
+        <v>1990</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1654</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E31">
+        <v>1992</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1762</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>935</v>
+      </c>
+      <c r="B32">
+        <v>1990</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1654</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E32">
+        <v>1992</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1776</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>937</v>
+      </c>
+      <c r="B33">
+        <v>1993</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1657</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E33">
+        <v>1994</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1771</v>
+      </c>
+      <c r="G33" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>945</v>
+      </c>
+      <c r="B34">
+        <v>1993</v>
+      </c>
+      <c r="C34" t="s">
+        <v>313</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E34">
+        <v>1994</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1773</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>946</v>
+      </c>
+      <c r="B35">
+        <v>1993</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1666</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E35">
+        <v>1994</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1777</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>946</v>
+      </c>
+      <c r="B36">
+        <v>1993</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1666</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E36">
+        <v>1994</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1771</v>
+      </c>
+      <c r="G36" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>947</v>
+      </c>
+      <c r="B37">
+        <v>1993</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1670</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E37">
+        <v>1993</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1769</v>
+      </c>
+      <c r="G37" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>948</v>
+      </c>
+      <c r="B38">
+        <v>1993</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1672</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E38">
+        <v>1994</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1778</v>
+      </c>
+      <c r="G38" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>948</v>
+      </c>
+      <c r="B39">
+        <v>1993</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1672</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E39">
+        <v>1994</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1779</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>948</v>
+      </c>
+      <c r="B40">
+        <v>1993</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1672</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E40">
+        <v>1994</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1773</v>
+      </c>
+      <c r="G40" t="s">
         <v>1751</v>
       </c>
     </row>
@@ -15431,7 +16442,7 @@
   <dimension ref="A1:D577"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23532,7 +24543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0DE966-0048-47B9-BC2F-FA793478304B}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add CREW_AWARD and MOVIE_AWARD
</commit_message>
<xml_diff>
--- a/movies.xlsx
+++ b/movies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johann Wagner\Documents\GitHub\comp2400\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0579696D-A9B9-44A4-8779-E384413B608A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94628702-42C5-4B48-8F7D-A1FB820364F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24800" windowHeight="14620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24800" windowHeight="14620" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MOVIE" sheetId="3" r:id="rId1"/>
@@ -26,6 +26,8 @@
     <sheet name="WRITER_AWARD" sheetId="12" r:id="rId11"/>
     <sheet name="DIRECTOR_AWARD" sheetId="13" r:id="rId12"/>
     <sheet name="ACTOR_AWARD" sheetId="14" r:id="rId13"/>
+    <sheet name="CREW_AWARD" sheetId="15" r:id="rId14"/>
+    <sheet name="MOVIE_AWARD" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5413" uniqueCount="1780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5670" uniqueCount="1793">
   <si>
     <t>id</t>
   </si>
@@ -5388,6 +5390,45 @@
   </si>
   <si>
     <t>BestActorSupporting</t>
+  </si>
+  <si>
+    <t>BestOriginalMusicScore</t>
+  </si>
+  <si>
+    <t>SoundTrack</t>
+  </si>
+  <si>
+    <t>SetDecorating</t>
+  </si>
+  <si>
+    <t>BestCostumeDesign</t>
+  </si>
+  <si>
+    <t>BestCinematography</t>
+  </si>
+  <si>
+    <t>bestpicture</t>
+  </si>
+  <si>
+    <t>bestfilm</t>
+  </si>
+  <si>
+    <t>BestMotionPictureDrama</t>
+  </si>
+  <si>
+    <t>BestFilm</t>
+  </si>
+  <si>
+    <t>BestForeignLanguageFilm</t>
+  </si>
+  <si>
+    <t>BestFilmnotintheEnglishLanguage</t>
+  </si>
+  <si>
+    <t>ForeignLanguageFilmoftheYear</t>
+  </si>
+  <si>
+    <t>WON</t>
   </si>
 </sst>
 </file>
@@ -16437,6 +16478,1410 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD97B548-E9EA-416B-9A1A-4B2E66CD99E6}">
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>896</v>
+      </c>
+      <c r="C1" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1742</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1743</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>209</v>
+      </c>
+      <c r="B2" t="s">
+        <v>991</v>
+      </c>
+      <c r="C2">
+        <v>1999</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E2">
+        <v>1999</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>205</v>
+      </c>
+      <c r="B3" t="s">
+        <v>991</v>
+      </c>
+      <c r="C3">
+        <v>1999</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E3">
+        <v>1999</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>206</v>
+      </c>
+      <c r="B4" t="s">
+        <v>991</v>
+      </c>
+      <c r="C4">
+        <v>1999</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E4">
+        <v>1999</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>207</v>
+      </c>
+      <c r="B5" t="s">
+        <v>991</v>
+      </c>
+      <c r="C5">
+        <v>1999</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E5">
+        <v>1999</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>208</v>
+      </c>
+      <c r="B6" t="s">
+        <v>991</v>
+      </c>
+      <c r="C6">
+        <v>1999</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E6">
+        <v>1999</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>980</v>
+      </c>
+      <c r="C7">
+        <v>1998</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E7">
+        <v>1998</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1140</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C8">
+        <v>1993</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E8">
+        <v>1993</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>306</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C9">
+        <v>1993</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E9">
+        <v>1993</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>307</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C10">
+        <v>1993</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E10">
+        <v>1993</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1083</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>307</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C11">
+        <v>1993</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E11">
+        <v>1994</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1083</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>306</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C12">
+        <v>1993</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E12">
+        <v>1994</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>325</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C13">
+        <v>1979</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E13">
+        <v>1979</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1780</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>348</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C14">
+        <v>1992</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E14">
+        <v>1993</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1083</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>349</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C15">
+        <v>1992</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E15">
+        <v>1993</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>348</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C16">
+        <v>1992</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E16">
+        <v>1992</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1083</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>349</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C17">
+        <v>1992</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E17">
+        <v>1992</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>347</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C18">
+        <v>1992</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E18">
+        <v>1992</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>547</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C19">
+        <v>1979</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E19">
+        <v>1980</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1086</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>546</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C20">
+        <v>1979</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E20">
+        <v>1980</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1083</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>545</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C21">
+        <v>1979</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E21">
+        <v>1980</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1781</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>562</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C22">
+        <v>1986</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E22">
+        <v>1987</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>563</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C23">
+        <v>1986</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E23">
+        <v>1987</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>564</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C24">
+        <v>1986</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E24">
+        <v>1987</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>979</v>
+      </c>
+      <c r="C25">
+        <v>1997</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E25">
+        <v>1998</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1782</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>979</v>
+      </c>
+      <c r="C26">
+        <v>1997</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E26">
+        <v>1998</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>979</v>
+      </c>
+      <c r="C27">
+        <v>1997</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E27">
+        <v>1998</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>979</v>
+      </c>
+      <c r="C28">
+        <v>1997</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E28">
+        <v>1998</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>979</v>
+      </c>
+      <c r="C29">
+        <v>1997</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E29">
+        <v>1998</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>979</v>
+      </c>
+      <c r="C30">
+        <v>1997</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E30">
+        <v>1998</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>979</v>
+      </c>
+      <c r="C31">
+        <v>1997</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E31">
+        <v>1998</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>979</v>
+      </c>
+      <c r="C32">
+        <v>1997</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E32">
+        <v>1998</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1090</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>979</v>
+      </c>
+      <c r="C33">
+        <v>1997</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E33">
+        <v>1998</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G33" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>1013</v>
+      </c>
+      <c r="B34" t="s">
+        <v>917</v>
+      </c>
+      <c r="C34">
+        <v>1994</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E34">
+        <v>1995</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1783</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>1059</v>
+      </c>
+      <c r="B35" t="s">
+        <v>476</v>
+      </c>
+      <c r="C35">
+        <v>1992</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E35">
+        <v>1993</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1783</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>1130</v>
+      </c>
+      <c r="B36" t="s">
+        <v>935</v>
+      </c>
+      <c r="C36">
+        <v>1990</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E36">
+        <v>1991</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1783</v>
+      </c>
+      <c r="G36" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>1128</v>
+      </c>
+      <c r="B37" t="s">
+        <v>935</v>
+      </c>
+      <c r="C37">
+        <v>1990</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E37">
+        <v>1992</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1784</v>
+      </c>
+      <c r="G37" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>1130</v>
+      </c>
+      <c r="B38" t="s">
+        <v>935</v>
+      </c>
+      <c r="C38">
+        <v>1990</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E38">
+        <v>1992</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1783</v>
+      </c>
+      <c r="G38" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C9CBE7E-C240-4786-923F-73C5F1315AB2}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>896</v>
+      </c>
+      <c r="B1" t="s">
+        <v>897</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1742</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1743</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B2">
+        <v>2000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D2">
+        <v>2001</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1785</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B3">
+        <v>2000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D3">
+        <v>2001</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1786</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B4">
+        <v>2000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D4">
+        <v>2001</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1787</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B5">
+        <v>2000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D5">
+        <v>2000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1788</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>980</v>
+      </c>
+      <c r="B6">
+        <v>1998</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D6">
+        <v>1999</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1786</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>984</v>
+      </c>
+      <c r="B7">
+        <v>1999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D7">
+        <v>2000</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1786</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>982</v>
+      </c>
+      <c r="B8">
+        <v>1982</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D8">
+        <v>1983</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1786</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>984</v>
+      </c>
+      <c r="B9">
+        <v>1999</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D9">
+        <v>1999</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1785</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B10">
+        <v>1993</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D10">
+        <v>1993</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1786</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B11">
+        <v>1992</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D11">
+        <v>1992</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1786</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B12">
+        <v>1992</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D12">
+        <v>1993</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1786</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>979</v>
+      </c>
+      <c r="B13">
+        <v>1997</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D13">
+        <v>1998</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1785</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>932</v>
+      </c>
+      <c r="B14">
+        <v>1990</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D14">
+        <v>1991</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>934</v>
+      </c>
+      <c r="B15">
+        <v>1991</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D15">
+        <v>1992</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>934</v>
+      </c>
+      <c r="B16">
+        <v>1991</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D16">
+        <v>1993</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1790</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>934</v>
+      </c>
+      <c r="B17">
+        <v>1991</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D17">
+        <v>1992</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>935</v>
+      </c>
+      <c r="B18">
+        <v>1990</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D18">
+        <v>1991</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>935</v>
+      </c>
+      <c r="B19">
+        <v>1990</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D19">
+        <v>1992</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1790</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>935</v>
+      </c>
+      <c r="B20">
+        <v>1990</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D20">
+        <v>1991</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>935</v>
+      </c>
+      <c r="B21">
+        <v>1990</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D21">
+        <v>1991</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1791</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>947</v>
+      </c>
+      <c r="B22">
+        <v>1993</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D22">
+        <v>1994</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>947</v>
+      </c>
+      <c r="B23">
+        <v>1993</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D23">
+        <v>1994</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1790</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>947</v>
+      </c>
+      <c r="B24">
+        <v>1993</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D24">
+        <v>1994</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>947</v>
+      </c>
+      <c r="B25">
+        <v>1993</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D25">
+        <v>1993</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1792</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D577"/>
@@ -24543,7 +25988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0DE966-0048-47B9-BC2F-FA793478304B}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>